<commit_message>
Added visualization to the MILP version
</commit_message>
<xml_diff>
--- a/Pyomo/MILP_v1/Input_Files/InputData34_test.xlsx
+++ b/Pyomo/MILP_v1/Input_Files/InputData34_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip Forro\PycharmProjects\MasterThesis\Pyomo\MILP_v1\Input_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAB7A01-8091-42FC-A532-2DBF21298588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2447CC6-5CA8-436D-BA2C-A7FADF13870B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="890" activeTab="9" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="890" activeTab="10" xr2:uid="{C29AC206-A880-42C7-97CB-0C3D79BA6B73}"/>
   </bookViews>
   <sheets>
     <sheet name="LineData" sheetId="3" r:id="rId1"/>
@@ -737,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D19BE1F-7FF3-4617-8CC4-990DA12B4F3A}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -804,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C358DC-12EF-4E1A-B9B4-66615C268D13}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>